<commit_message>
Added turnout function and vignette. Updated other vignettes.
</commit_message>
<xml_diff>
--- a/inst/extdata/CharterResults.xlsx
+++ b/inst/extdata/CharterResults.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sharon\My Documents Data Drive\R\elections2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DBB7D5-E337-40D3-AE9E-873924FF75BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C002A7-6424-479C-9A36-6E241EB4CC61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8685" yWindow="1020" windowWidth="13785" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8220" yWindow="1425" windowWidth="17475" windowHeight="13410" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Charter" sheetId="2" r:id="rId3"/>
+    <sheet name="Turnout" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Total</t>
   </si>
@@ -56,12 +57,18 @@
   <si>
     <t>Precinct</t>
   </si>
+  <si>
+    <t>Turnout</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +94,33 @@
       <name val="Arial Bold Italic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial Bold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial Bold"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -119,6 +153,11 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -797,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:T8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1541,4 +1580,175 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C6F89A-FEAB-453D-BE10-AB43AE952E99}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14">
+        <v>0.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>